<commit_message>
add cover for the deep methods for CV
</commit_message>
<xml_diff>
--- a/training_schedule.xlsx
+++ b/training_schedule.xlsx
@@ -1,23 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\CV_training\CV_training\CV_training\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sus85\OneDrive\Desktop\CV\CV_training\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FDED91-BAAF-4701-AE32-D49A6F11FC08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10710" windowHeight="4220"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -123,12 +135,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -438,18 +450,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.9140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -476,7 +488,7 @@
       </c>
       <c r="D2">
         <f>SUM(D3)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -486,6 +498,9 @@
       <c r="C3">
         <v>0.5</v>
       </c>
+      <c r="D3">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -497,7 +512,7 @@
       </c>
       <c r="D5">
         <f>SUM(D6:D11)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -507,6 +522,9 @@
       <c r="C6">
         <v>1</v>
       </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
@@ -515,6 +533,9 @@
       <c r="C7">
         <v>2</v>
       </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
@@ -531,6 +552,9 @@
       <c r="C9">
         <v>1</v>
       </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
@@ -548,7 +572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>